<commit_message>
Errno 2 for Path_setup/CA_imports.csv
</commit_message>
<xml_diff>
--- a/Stochastic_engine/PNW_hydro/PNW_hydro_daily.xlsx
+++ b/Stochastic_engine/PNW_hydro/PNW_hydro_daily.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>PNW</t>
   </si>
@@ -24,22 +23,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,26 +57,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -361,18 +373,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
@@ -380,2926 +386,2926 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>286958.3826888078</v>
+      <c r="B2">
+        <v>360845.5911344764</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>313162.9500301483</v>
+      <c r="B3">
+        <v>304736.0418538008</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>307383.8672302283</v>
+      <c r="B4">
+        <v>312402.5744275864</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>302832.5819380729</v>
+      <c r="B5">
+        <v>316638.1469426657</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>303055.0421082866</v>
+      <c r="B6">
+        <v>348272.4215004222</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>297771.9957271108</v>
+      <c r="B7">
+        <v>382637.1940829552</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>304751.5574888405</v>
+      <c r="B8">
+        <v>388058.4061800578</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
-        <v>306156.6031854475</v>
+      <c r="B9">
+        <v>411165.2970455751</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>312444.3486298018</v>
+      <c r="B10">
+        <v>421164.7516623765</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>311588.801171537</v>
+      <c r="B11">
+        <v>411223.8495270232</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
-        <v>307287.6804918933</v>
+      <c r="B12">
+        <v>434892.3663751524</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
-        <v>298718.0075837805</v>
+      <c r="B13">
+        <v>436102.8057459489</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="n">
-        <v>301689.8466543751</v>
+      <c r="B14">
+        <v>413475.8969846909</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="n">
-        <v>292501.111110451</v>
+      <c r="B15">
+        <v>415951.0035452747</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="n">
-        <v>301521.0533524943</v>
+      <c r="B16">
+        <v>390345.6782119777</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
-        <v>325058.2756290578</v>
+      <c r="B17">
+        <v>365321.4357459462</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="n">
-        <v>318424.7294607092</v>
+      <c r="B18">
+        <v>346594.8136706604</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="n">
-        <v>321798.9066456861</v>
+      <c r="B19">
+        <v>343853.2842360042</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="n">
-        <v>310240.5755740961</v>
+      <c r="B20">
+        <v>339697.5875914758</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="n">
-        <v>321393.3094344226</v>
+      <c r="B21">
+        <v>339355.9039934391</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="n">
-        <v>367987.8814759384</v>
+      <c r="B22">
+        <v>336876.8014487805</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="n">
-        <v>387321.5703117486</v>
+      <c r="B23">
+        <v>376999.0024865718</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="n">
-        <v>393416.8258958092</v>
+      <c r="B24">
+        <v>377731.3631791678</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="n">
-        <v>388750.9867265229</v>
+      <c r="B25">
+        <v>389915.8336736226</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="n">
-        <v>399057.7369751186</v>
+      <c r="B26">
+        <v>398781.9343538179</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="n">
-        <v>394044.9589499517</v>
+      <c r="B27">
+        <v>394410.644660852</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="n">
-        <v>382238.2431904819</v>
+      <c r="B28">
+        <v>388056.7035419751</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="n">
-        <v>363889.1785648675</v>
+      <c r="B29">
+        <v>414179.5080753333</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" t="n">
-        <v>356445.0767414129</v>
+      <c r="B30">
+        <v>412174.8507482873</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" t="n">
-        <v>362680.7927580342</v>
+      <c r="B31">
+        <v>400783.3184595602</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" t="n">
-        <v>367503.1966037708</v>
+      <c r="B32">
+        <v>394377.5591078613</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" t="n">
-        <v>365020.2260485952</v>
+      <c r="B33">
+        <v>389984.4111965815</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" t="n">
-        <v>355377.9556077471</v>
+      <c r="B34">
+        <v>375901.4828404218</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" t="n">
-        <v>384077.3121247956</v>
+      <c r="B35">
+        <v>362615.5380639629</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" t="n">
-        <v>383097.4812049224</v>
+      <c r="B36">
+        <v>341104.4335497106</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" t="n">
-        <v>405683.3791368561</v>
+      <c r="B37">
+        <v>331897.1179534797</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" t="n">
-        <v>396957.8431902783</v>
+      <c r="B38">
+        <v>342934.4654320527</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" t="n">
-        <v>386548.1300842958</v>
+      <c r="B39">
+        <v>350910.5670495433</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" t="n">
-        <v>372361.7109940399</v>
+      <c r="B40">
+        <v>351244.3900936371</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" t="n">
-        <v>358012.4186610748</v>
+      <c r="B41">
+        <v>346223.0726807831</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" t="n">
-        <v>354231.1951476912</v>
+      <c r="B42">
+        <v>344439.3982836059</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" t="n">
-        <v>355007.2118891011</v>
+      <c r="B43">
+        <v>360443.0947901381</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" t="n">
-        <v>356050.8570536628</v>
+      <c r="B44">
+        <v>369559.4284324406</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" t="n">
-        <v>351197.826119862</v>
+      <c r="B45">
+        <v>392332.0751643137</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" t="n">
-        <v>343862.2319649634</v>
+      <c r="B46">
+        <v>388725.703853919</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" t="n">
-        <v>344137.7805636049</v>
+      <c r="B47">
+        <v>387934.5418842331</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" t="n">
-        <v>335763.9285645216</v>
+      <c r="B48">
+        <v>389632.0288099989</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" t="n">
-        <v>328708.4943932634</v>
+      <c r="B49">
+        <v>401112.0296778122</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" t="n">
-        <v>339619.3094314117</v>
+      <c r="B50">
+        <v>440262.4747788454</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" t="n">
-        <v>401125.9526819309</v>
+      <c r="B51">
+        <v>445671.9849667194</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" t="n">
-        <v>441078.4985093106</v>
+      <c r="B52">
+        <v>458710.2856627915</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" t="n">
-        <v>476130.6579241037</v>
+      <c r="B53">
+        <v>457184.7571209607</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" t="n">
-        <v>517977.9382656785</v>
+      <c r="B54">
+        <v>451332.1807247838</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" t="n">
-        <v>525479.939950446</v>
+      <c r="B55">
+        <v>447510.1762081419</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" t="n">
-        <v>517509.4657025951</v>
+      <c r="B56">
+        <v>439977.5726060454</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" t="n">
-        <v>527578.893752892</v>
+      <c r="B57">
+        <v>435615.4943052612</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" t="n">
-        <v>519983.9712532851</v>
+      <c r="B58">
+        <v>446904.450958693</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" t="n">
-        <v>509024.7066782232</v>
+      <c r="B59">
+        <v>453688.1440202061</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" t="n">
-        <v>465328.3557151774</v>
+      <c r="B60">
+        <v>443761.4999506631</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" t="n">
-        <v>469209.2521240507</v>
+      <c r="B61">
+        <v>460866.550550758</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" t="n">
-        <v>417897.6581391308</v>
+      <c r="B62">
+        <v>420021.2665875116</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" t="n">
-        <v>418139.3756927071</v>
+      <c r="B63">
+        <v>402926.2209942079</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" t="n">
-        <v>415993.9437067595</v>
+      <c r="B64">
+        <v>411088.8328121532</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" t="n">
-        <v>412200.6299606238</v>
+      <c r="B65">
+        <v>415647.4641786826</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" t="n">
-        <v>425800.4879515762</v>
+      <c r="B66">
+        <v>427121.0639531151</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" t="n">
-        <v>439306.5286962829</v>
+      <c r="B67">
+        <v>438261.4622757004</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" t="n">
-        <v>436118.9677297577</v>
+      <c r="B68">
+        <v>446641.4577628482</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" t="n">
-        <v>436742.7189058148</v>
+      <c r="B69">
+        <v>455069.5054200666</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" t="n">
-        <v>417999.1016123589</v>
+      <c r="B70">
+        <v>509165.5759632299</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" t="n">
-        <v>402896.0653776719</v>
+      <c r="B71">
+        <v>525974.6750356668</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" t="n">
-        <v>385740.6698555979</v>
+      <c r="B72">
+        <v>527499.7849147834</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="1">
         <v>71</v>
       </c>
-      <c r="B73" t="n">
-        <v>370512.0715783811</v>
+      <c r="B73">
+        <v>529227.6423369047</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" t="n">
-        <v>378465.2616763684</v>
+      <c r="B74">
+        <v>531908.1740864638</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" t="n">
-        <v>373960.6218523822</v>
+      <c r="B75">
+        <v>527500.0590212874</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B76" t="n">
-        <v>405177.4628102286</v>
+      <c r="B76">
+        <v>519259.8712450856</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B77" t="n">
-        <v>453878.0843759428</v>
+      <c r="B77">
+        <v>511455.323905853</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" t="n">
-        <v>445554.9251303387</v>
+      <c r="B78">
+        <v>499592.3189076044</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" t="n">
-        <v>434367.9416735333</v>
+      <c r="B79">
+        <v>485965.4472500755</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" t="n">
-        <v>420077.1833479523</v>
+      <c r="B80">
+        <v>472579.1889543937</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" t="n">
-        <v>414236.8641746935</v>
+      <c r="B81">
+        <v>458724.5712750112</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" t="n">
-        <v>414818.5225024776</v>
+      <c r="B82">
+        <v>458308.0174193699</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" t="n">
-        <v>421925.5833834488</v>
+      <c r="B83">
+        <v>451528.7971527735</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" t="n">
-        <v>421900.0179421975</v>
+      <c r="B84">
+        <v>438168.5857217099</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85" t="n">
-        <v>373700.525774257</v>
+      <c r="B85">
+        <v>393811.1254755015</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="1">
         <v>84</v>
       </c>
-      <c r="B86" t="n">
-        <v>396492.9104083541</v>
+      <c r="B86">
+        <v>403811.4784827326</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" t="n">
-        <v>399061.5278638517</v>
+      <c r="B87">
+        <v>387910.8837785505</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88" t="n">
-        <v>403103.3245555679</v>
+      <c r="B88">
+        <v>384390.6318572317</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89" t="n">
-        <v>407449.6928243196</v>
+      <c r="B89">
+        <v>376179.9500824576</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" t="n">
-        <v>409329.7135207698</v>
+      <c r="B90">
+        <v>417947.6939742673</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" t="n">
-        <v>416048.9035805674</v>
+      <c r="B91">
+        <v>419657.6935557085</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92" t="n">
-        <v>381521.6413976901</v>
+      <c r="B92">
+        <v>405262.7224076128</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93" t="n">
-        <v>331050.6393488969</v>
+      <c r="B93">
+        <v>358838.6647078344</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94" t="n">
-        <v>324801.1339430276</v>
+      <c r="B94">
+        <v>359122.0661331314</v>
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" t="n">
-        <v>344554.1720834773</v>
+      <c r="B95">
+        <v>351407.0296532008</v>
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" t="n">
-        <v>330623.013894601</v>
+      <c r="B96">
+        <v>336842.0764526594</v>
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="1">
         <v>95</v>
       </c>
-      <c r="B97" t="n">
-        <v>354723.0276003429</v>
+      <c r="B97">
+        <v>334769.9355369408</v>
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" t="n">
-        <v>353907.7494003526</v>
+      <c r="B98">
+        <v>337137.2249865353</v>
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99" t="n">
-        <v>341430.8893728139</v>
+      <c r="B99">
+        <v>337807.3205431438</v>
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100" t="n">
-        <v>319771.3288275141</v>
+      <c r="B100">
+        <v>334579.7580159211</v>
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" t="n">
-        <v>309625.5702406288</v>
+      <c r="B101">
+        <v>342243.2032180532</v>
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" t="n">
-        <v>318335.5621934464</v>
+      <c r="B102">
+        <v>341287.4682218048</v>
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="1">
         <v>101</v>
       </c>
-      <c r="B103" t="n">
-        <v>309700.5656655258</v>
+      <c r="B103">
+        <v>329898.8484220401</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104" t="n">
-        <v>317802.5693932562</v>
+      <c r="B104">
+        <v>310644.7941841654</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105" t="n">
-        <v>331361.2401719908</v>
+      <c r="B105">
+        <v>302977.4093872103</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106" t="n">
-        <v>319829.7069840727</v>
+      <c r="B106">
+        <v>303161.7968238351</v>
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107" t="n">
-        <v>319017.0876113623</v>
+      <c r="B107">
+        <v>292728.4040123668</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="1">
         <v>106</v>
       </c>
-      <c r="B108" t="n">
-        <v>315198.1716823228</v>
+      <c r="B108">
+        <v>284970.3633092481</v>
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" t="n">
-        <v>306205.8798630918</v>
+      <c r="B109">
+        <v>290663.8310994279</v>
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="1">
         <v>108</v>
       </c>
-      <c r="B110" t="n">
-        <v>303521.213343805</v>
+      <c r="B110">
+        <v>313170.9376983867</v>
       </c>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="1">
         <v>109</v>
       </c>
-      <c r="B111" t="n">
-        <v>303450.940084226</v>
+      <c r="B111">
+        <v>333666.1403418515</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="1">
         <v>110</v>
       </c>
-      <c r="B112" t="n">
-        <v>287726.398824239</v>
+      <c r="B112">
+        <v>361280.9167311262</v>
       </c>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="1">
         <v>111</v>
       </c>
-      <c r="B113" t="n">
-        <v>276390.2233660801</v>
+      <c r="B113">
+        <v>390289.0841787281</v>
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" t="n">
-        <v>282418.5584028049</v>
+      <c r="B114">
+        <v>420463.1644419847</v>
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="1">
         <v>113</v>
       </c>
-      <c r="B115" t="n">
-        <v>271833.5830253747</v>
+      <c r="B115">
+        <v>457673.5889056582</v>
       </c>
     </row>
     <row r="116" spans="1:2">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="1">
         <v>114</v>
       </c>
-      <c r="B116" t="n">
-        <v>271327.9155510381</v>
+      <c r="B116">
+        <v>493977.7473274866</v>
       </c>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="1">
         <v>115</v>
       </c>
-      <c r="B117" t="n">
-        <v>267883.0969159569</v>
+      <c r="B117">
+        <v>507005.6545082584</v>
       </c>
     </row>
     <row r="118" spans="1:2">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="1">
         <v>116</v>
       </c>
-      <c r="B118" t="n">
-        <v>260833.0107182817</v>
+      <c r="B118">
+        <v>506439.2243213222</v>
       </c>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="1">
         <v>117</v>
       </c>
-      <c r="B119" t="n">
-        <v>268497.4309600291</v>
+      <c r="B119">
+        <v>506050.2327974146</v>
       </c>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="1">
         <v>118</v>
       </c>
-      <c r="B120" t="n">
-        <v>278291.3497549043</v>
+      <c r="B120">
+        <v>489286.1776722127</v>
       </c>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="B121" t="n">
-        <v>298458.5388052508</v>
+      <c r="B121">
+        <v>480526.2603488206</v>
       </c>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="B122" t="n">
-        <v>201659.603575348</v>
+      <c r="B122">
+        <v>277214.5673398314</v>
       </c>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" t="n">
-        <v>211574.9890761334</v>
+      <c r="B123">
+        <v>262367.7562298108</v>
       </c>
     </row>
     <row r="124" spans="1:2">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="1">
         <v>122</v>
       </c>
-      <c r="B124" t="n">
-        <v>216096.6874762063</v>
+      <c r="B124">
+        <v>260699.1202023877</v>
       </c>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="1">
         <v>123</v>
       </c>
-      <c r="B125" t="n">
-        <v>232060.3819440021</v>
+      <c r="B125">
+        <v>258457.9491218527</v>
       </c>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="1">
         <v>124</v>
       </c>
-      <c r="B126" t="n">
-        <v>239984.1637731457</v>
+      <c r="B126">
+        <v>266273.5389532291</v>
       </c>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="1">
         <v>125</v>
       </c>
-      <c r="B127" t="n">
-        <v>238739.4574795795</v>
+      <c r="B127">
+        <v>285171.1573002017</v>
       </c>
     </row>
     <row r="128" spans="1:2">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="B128" t="n">
-        <v>231721.8846084866</v>
+      <c r="B128">
+        <v>301854.6321716918</v>
       </c>
     </row>
     <row r="129" spans="1:2">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="1">
         <v>127</v>
       </c>
-      <c r="B129" t="n">
-        <v>226117.3699568681</v>
+      <c r="B129">
+        <v>320572.4351833767</v>
       </c>
     </row>
     <row r="130" spans="1:2">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="1">
         <v>128</v>
       </c>
-      <c r="B130" t="n">
-        <v>222440.7453787772</v>
+      <c r="B130">
+        <v>322094.1737089807</v>
       </c>
     </row>
     <row r="131" spans="1:2">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="1">
         <v>129</v>
       </c>
-      <c r="B131" t="n">
-        <v>227474.0009756871</v>
+      <c r="B131">
+        <v>299487.1171811062</v>
       </c>
     </row>
     <row r="132" spans="1:2">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" t="n">
-        <v>235565.7024938978</v>
+      <c r="B132">
+        <v>279502.7384469077</v>
       </c>
     </row>
     <row r="133" spans="1:2">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" t="n">
-        <v>247195.2816526776</v>
+      <c r="B133">
+        <v>250567.7392301491</v>
       </c>
     </row>
     <row r="134" spans="1:2">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="1">
         <v>132</v>
       </c>
-      <c r="B134" t="n">
-        <v>255825.7691863721</v>
+      <c r="B134">
+        <v>239736.8023129301</v>
       </c>
     </row>
     <row r="135" spans="1:2">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="1">
         <v>133</v>
       </c>
-      <c r="B135" t="n">
-        <v>265987.1085490803</v>
+      <c r="B135">
+        <v>243384.1982305916</v>
       </c>
     </row>
     <row r="136" spans="1:2">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="1">
         <v>134</v>
       </c>
-      <c r="B136" t="n">
-        <v>268290.1743288806</v>
+      <c r="B136">
+        <v>239581.3759433459</v>
       </c>
     </row>
     <row r="137" spans="1:2">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="1">
         <v>135</v>
       </c>
-      <c r="B137" t="n">
-        <v>331585.3279776216</v>
+      <c r="B137">
+        <v>246726.7511912522</v>
       </c>
     </row>
     <row r="138" spans="1:2">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="1">
         <v>136</v>
       </c>
-      <c r="B138" t="n">
-        <v>309548.929211035</v>
+      <c r="B138">
+        <v>244705.5309080131</v>
       </c>
     </row>
     <row r="139" spans="1:2">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="1">
         <v>137</v>
       </c>
-      <c r="B139" t="n">
-        <v>384628.1708094378</v>
+      <c r="B139">
+        <v>246653.1233075094</v>
       </c>
     </row>
     <row r="140" spans="1:2">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="B140" t="n">
-        <v>362795.128617359</v>
+      <c r="B140">
+        <v>250604.6064423972</v>
       </c>
     </row>
     <row r="141" spans="1:2">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="1">
         <v>139</v>
       </c>
-      <c r="B141" t="n">
-        <v>513155.3887403218</v>
+      <c r="B141">
+        <v>341987.6275851741</v>
       </c>
     </row>
     <row r="142" spans="1:2">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="1">
         <v>140</v>
       </c>
-      <c r="B142" t="n">
-        <v>507977.3771936537</v>
+      <c r="B142">
+        <v>443525.0816959462</v>
       </c>
     </row>
     <row r="143" spans="1:2">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="1">
         <v>141</v>
       </c>
-      <c r="B143" t="n">
-        <v>533793.8757067025</v>
+      <c r="B143">
+        <v>446649.4340953064</v>
       </c>
     </row>
     <row r="144" spans="1:2">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="1">
         <v>142</v>
       </c>
-      <c r="B144" t="n">
-        <v>513168.7048670122</v>
+      <c r="B144">
+        <v>502952.2761463284</v>
       </c>
     </row>
     <row r="145" spans="1:2">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="1">
         <v>143</v>
       </c>
-      <c r="B145" t="n">
-        <v>540390.7944019332</v>
+      <c r="B145">
+        <v>537197.6043692972</v>
       </c>
     </row>
     <row r="146" spans="1:2">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="1">
         <v>144</v>
       </c>
-      <c r="B146" t="n">
-        <v>518964.5262213209</v>
+      <c r="B146">
+        <v>539277.2786868642</v>
       </c>
     </row>
     <row r="147" spans="1:2">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="1">
         <v>145</v>
       </c>
-      <c r="B147" t="n">
-        <v>535419.2973185468</v>
+      <c r="B147">
+        <v>556125.4018061969</v>
       </c>
     </row>
     <row r="148" spans="1:2">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="1">
         <v>146</v>
       </c>
-      <c r="B148" t="n">
-        <v>523083.091376166</v>
+      <c r="B148">
+        <v>559281.1345053421</v>
       </c>
     </row>
     <row r="149" spans="1:2">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="1">
         <v>147</v>
       </c>
-      <c r="B149" t="n">
-        <v>537859.6375476375</v>
+      <c r="B149">
+        <v>558260.3341907357</v>
       </c>
     </row>
     <row r="150" spans="1:2">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="1">
         <v>148</v>
       </c>
-      <c r="B150" t="n">
-        <v>509513.9017184209</v>
+      <c r="B150">
+        <v>557733.5818746992</v>
       </c>
     </row>
     <row r="151" spans="1:2">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="1">
         <v>149</v>
       </c>
-      <c r="B151" t="n">
-        <v>533976.463453939</v>
+      <c r="B151">
+        <v>557748.0879054922</v>
       </c>
     </row>
     <row r="152" spans="1:2">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="1">
         <v>150</v>
       </c>
-      <c r="B152" t="n">
-        <v>509798.3683698811</v>
+      <c r="B152">
+        <v>559693.5755611372</v>
       </c>
     </row>
     <row r="153" spans="1:2">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="1">
         <v>151</v>
       </c>
-      <c r="B153" t="n">
-        <v>539325.6566207178</v>
+      <c r="B153">
+        <v>561175.8214472065</v>
       </c>
     </row>
     <row r="154" spans="1:2">
-      <c r="A154" s="1" t="n">
+      <c r="A154" s="1">
         <v>152</v>
       </c>
-      <c r="B154" t="n">
-        <v>523478.5968257517</v>
+      <c r="B154">
+        <v>543581.0288724895</v>
       </c>
     </row>
     <row r="155" spans="1:2">
-      <c r="A155" s="1" t="n">
+      <c r="A155" s="1">
         <v>153</v>
       </c>
-      <c r="B155" t="n">
-        <v>555877.6164886003</v>
+      <c r="B155">
+        <v>564533.1433583163</v>
       </c>
     </row>
     <row r="156" spans="1:2">
-      <c r="A156" s="1" t="n">
+      <c r="A156" s="1">
         <v>154</v>
       </c>
-      <c r="B156" t="n">
-        <v>555499.9890019033</v>
+      <c r="B156">
+        <v>557491.7522613913</v>
       </c>
     </row>
     <row r="157" spans="1:2">
-      <c r="A157" s="1" t="n">
+      <c r="A157" s="1">
         <v>155</v>
       </c>
-      <c r="B157" t="n">
-        <v>557114.7314511912</v>
+      <c r="B157">
+        <v>567535.7823872259</v>
       </c>
     </row>
     <row r="158" spans="1:2">
-      <c r="A158" s="1" t="n">
+      <c r="A158" s="1">
         <v>156</v>
       </c>
-      <c r="B158" t="n">
-        <v>561690.4747962769</v>
+      <c r="B158">
+        <v>567190.5847945481</v>
       </c>
     </row>
     <row r="159" spans="1:2">
-      <c r="A159" s="1" t="n">
+      <c r="A159" s="1">
         <v>157</v>
       </c>
-      <c r="B159" t="n">
-        <v>557798.9073321095</v>
+      <c r="B159">
+        <v>565351.6462590805</v>
       </c>
     </row>
     <row r="160" spans="1:2">
-      <c r="A160" s="1" t="n">
+      <c r="A160" s="1">
         <v>158</v>
       </c>
-      <c r="B160" t="n">
-        <v>552167.3486493045</v>
+      <c r="B160">
+        <v>564296.6229315159</v>
       </c>
     </row>
     <row r="161" spans="1:2">
-      <c r="A161" s="1" t="n">
+      <c r="A161" s="1">
         <v>159</v>
       </c>
-      <c r="B161" t="n">
-        <v>563784.2710982064</v>
+      <c r="B161">
+        <v>564556.0457094974</v>
       </c>
     </row>
     <row r="162" spans="1:2">
-      <c r="A162" s="1" t="n">
+      <c r="A162" s="1">
         <v>160</v>
       </c>
-      <c r="B162" t="n">
-        <v>554613.5217702652</v>
+      <c r="B162">
+        <v>564798.6337784164</v>
       </c>
     </row>
     <row r="163" spans="1:2">
-      <c r="A163" s="1" t="n">
+      <c r="A163" s="1">
         <v>161</v>
       </c>
-      <c r="B163" t="n">
-        <v>556340.9348887394</v>
+      <c r="B163">
+        <v>566204.1850756126</v>
       </c>
     </row>
     <row r="164" spans="1:2">
-      <c r="A164" s="1" t="n">
+      <c r="A164" s="1">
         <v>162</v>
       </c>
-      <c r="B164" t="n">
-        <v>547607.5846589867</v>
+      <c r="B164">
+        <v>566311.5902544189</v>
       </c>
     </row>
     <row r="165" spans="1:2">
-      <c r="A165" s="1" t="n">
+      <c r="A165" s="1">
         <v>163</v>
       </c>
-      <c r="B165" t="n">
-        <v>555490.6619454718</v>
+      <c r="B165">
+        <v>566146.0203034368</v>
       </c>
     </row>
     <row r="166" spans="1:2">
-      <c r="A166" s="1" t="n">
+      <c r="A166" s="1">
         <v>164</v>
       </c>
-      <c r="B166" t="n">
-        <v>546252.8261489148</v>
+      <c r="B166">
+        <v>561501.4952587812</v>
       </c>
     </row>
     <row r="167" spans="1:2">
-      <c r="A167" s="1" t="n">
+      <c r="A167" s="1">
         <v>165</v>
       </c>
-      <c r="B167" t="n">
-        <v>549457.4016722048</v>
+      <c r="B167">
+        <v>505158.0076420846</v>
       </c>
     </row>
     <row r="168" spans="1:2">
-      <c r="A168" s="1" t="n">
+      <c r="A168" s="1">
         <v>166</v>
       </c>
-      <c r="B168" t="n">
-        <v>537879.6915351172</v>
+      <c r="B168">
+        <v>523736.1384722714</v>
       </c>
     </row>
     <row r="169" spans="1:2">
-      <c r="A169" s="1" t="n">
+      <c r="A169" s="1">
         <v>167</v>
       </c>
-      <c r="B169" t="n">
-        <v>533751.6930879911</v>
+      <c r="B169">
+        <v>507426.4280543338</v>
       </c>
     </row>
     <row r="170" spans="1:2">
-      <c r="A170" s="1" t="n">
+      <c r="A170" s="1">
         <v>168</v>
       </c>
-      <c r="B170" t="n">
-        <v>509281.0401356531</v>
+      <c r="B170">
+        <v>528744.7546682103</v>
       </c>
     </row>
     <row r="171" spans="1:2">
-      <c r="A171" s="1" t="n">
+      <c r="A171" s="1">
         <v>169</v>
       </c>
-      <c r="B171" t="n">
-        <v>520721.8932652927</v>
+      <c r="B171">
+        <v>506742.6865969916</v>
       </c>
     </row>
     <row r="172" spans="1:2">
-      <c r="A172" s="1" t="n">
+      <c r="A172" s="1">
         <v>170</v>
       </c>
-      <c r="B172" t="n">
-        <v>514723.8525076683</v>
+      <c r="B172">
+        <v>513725.6645913102</v>
       </c>
     </row>
     <row r="173" spans="1:2">
-      <c r="A173" s="1" t="n">
+      <c r="A173" s="1">
         <v>171</v>
       </c>
-      <c r="B173" t="n">
-        <v>534290.7453425037</v>
+      <c r="B173">
+        <v>478696.1304638209</v>
       </c>
     </row>
     <row r="174" spans="1:2">
-      <c r="A174" s="1" t="n">
+      <c r="A174" s="1">
         <v>172</v>
       </c>
-      <c r="B174" t="n">
-        <v>509330.7947150621</v>
+      <c r="B174">
+        <v>482307.8604795506</v>
       </c>
     </row>
     <row r="175" spans="1:2">
-      <c r="A175" s="1" t="n">
+      <c r="A175" s="1">
         <v>173</v>
       </c>
-      <c r="B175" t="n">
-        <v>528037.8814360176</v>
+      <c r="B175">
+        <v>440129.5858659811</v>
       </c>
     </row>
     <row r="176" spans="1:2">
-      <c r="A176" s="1" t="n">
+      <c r="A176" s="1">
         <v>174</v>
       </c>
-      <c r="B176" t="n">
-        <v>530297.0192449127</v>
+      <c r="B176">
+        <v>473867.1452371317</v>
       </c>
     </row>
     <row r="177" spans="1:2">
-      <c r="A177" s="1" t="n">
+      <c r="A177" s="1">
         <v>175</v>
       </c>
-      <c r="B177" t="n">
-        <v>533606.634620299</v>
+      <c r="B177">
+        <v>476695.0915960427</v>
       </c>
     </row>
     <row r="178" spans="1:2">
-      <c r="A178" s="1" t="n">
+      <c r="A178" s="1">
         <v>176</v>
       </c>
-      <c r="B178" t="n">
-        <v>521312.4427389559</v>
+      <c r="B178">
+        <v>474780.1382125577</v>
       </c>
     </row>
     <row r="179" spans="1:2">
-      <c r="A179" s="1" t="n">
+      <c r="A179" s="1">
         <v>177</v>
       </c>
-      <c r="B179" t="n">
-        <v>528539.997235416</v>
+      <c r="B179">
+        <v>455651.4852364403</v>
       </c>
     </row>
     <row r="180" spans="1:2">
-      <c r="A180" s="1" t="n">
+      <c r="A180" s="1">
         <v>178</v>
       </c>
-      <c r="B180" t="n">
-        <v>518431.2221676114</v>
+      <c r="B180">
+        <v>459455.8358489608</v>
       </c>
     </row>
     <row r="181" spans="1:2">
-      <c r="A181" s="1" t="n">
+      <c r="A181" s="1">
         <v>179</v>
       </c>
-      <c r="B181" t="n">
-        <v>500493.6200017561</v>
+      <c r="B181">
+        <v>468991.9190822123</v>
       </c>
     </row>
     <row r="182" spans="1:2">
-      <c r="A182" s="1" t="n">
+      <c r="A182" s="1">
         <v>180</v>
       </c>
-      <c r="B182" t="n">
-        <v>451967.631254437</v>
+      <c r="B182">
+        <v>478137.622301045</v>
       </c>
     </row>
     <row r="183" spans="1:2">
-      <c r="A183" s="1" t="n">
+      <c r="A183" s="1">
         <v>181</v>
       </c>
-      <c r="B183" t="n">
-        <v>455614.4619767266</v>
+      <c r="B183">
+        <v>480567.4226336239</v>
       </c>
     </row>
     <row r="184" spans="1:2">
-      <c r="A184" s="1" t="n">
+      <c r="A184" s="1">
         <v>182</v>
       </c>
-      <c r="B184" t="n">
-        <v>379873.2132058894</v>
+      <c r="B184">
+        <v>495090.3663235181</v>
       </c>
     </row>
     <row r="185" spans="1:2">
-      <c r="A185" s="1" t="n">
+      <c r="A185" s="1">
         <v>183</v>
       </c>
-      <c r="B185" t="n">
-        <v>374180.766138844</v>
+      <c r="B185">
+        <v>517747.6766125533</v>
       </c>
     </row>
     <row r="186" spans="1:2">
-      <c r="A186" s="1" t="n">
+      <c r="A186" s="1">
         <v>184</v>
       </c>
-      <c r="B186" t="n">
-        <v>373000.5504918233</v>
+      <c r="B186">
+        <v>515629.0649422863</v>
       </c>
     </row>
     <row r="187" spans="1:2">
-      <c r="A187" s="1" t="n">
+      <c r="A187" s="1">
         <v>185</v>
       </c>
-      <c r="B187" t="n">
-        <v>370618.0010875</v>
+      <c r="B187">
+        <v>475194.801718686</v>
       </c>
     </row>
     <row r="188" spans="1:2">
-      <c r="A188" s="1" t="n">
+      <c r="A188" s="1">
         <v>186</v>
       </c>
-      <c r="B188" t="n">
-        <v>380415.6506699705</v>
+      <c r="B188">
+        <v>470403.3519037805</v>
       </c>
     </row>
     <row r="189" spans="1:2">
-      <c r="A189" s="1" t="n">
+      <c r="A189" s="1">
         <v>187</v>
       </c>
-      <c r="B189" t="n">
-        <v>388637.0249272548</v>
+      <c r="B189">
+        <v>465652.2632015444</v>
       </c>
     </row>
     <row r="190" spans="1:2">
-      <c r="A190" s="1" t="n">
+      <c r="A190" s="1">
         <v>188</v>
       </c>
-      <c r="B190" t="n">
-        <v>392838.1792196389</v>
+      <c r="B190">
+        <v>472509.1196060488</v>
       </c>
     </row>
     <row r="191" spans="1:2">
-      <c r="A191" s="1" t="n">
+      <c r="A191" s="1">
         <v>189</v>
       </c>
-      <c r="B191" t="n">
-        <v>373425.9698806929</v>
+      <c r="B191">
+        <v>444456.902887917</v>
       </c>
     </row>
     <row r="192" spans="1:2">
-      <c r="A192" s="1" t="n">
+      <c r="A192" s="1">
         <v>190</v>
       </c>
-      <c r="B192" t="n">
-        <v>355241.2455126468</v>
+      <c r="B192">
+        <v>444438.5199532512</v>
       </c>
     </row>
     <row r="193" spans="1:2">
-      <c r="A193" s="1" t="n">
+      <c r="A193" s="1">
         <v>191</v>
       </c>
-      <c r="B193" t="n">
-        <v>361006.4418018361</v>
+      <c r="B193">
+        <v>425795.0545150103</v>
       </c>
     </row>
     <row r="194" spans="1:2">
-      <c r="A194" s="1" t="n">
+      <c r="A194" s="1">
         <v>192</v>
       </c>
-      <c r="B194" t="n">
-        <v>364528.2993089429</v>
+      <c r="B194">
+        <v>429149.1172137957</v>
       </c>
     </row>
     <row r="195" spans="1:2">
-      <c r="A195" s="1" t="n">
+      <c r="A195" s="1">
         <v>193</v>
       </c>
-      <c r="B195" t="n">
-        <v>373273.9954254043</v>
+      <c r="B195">
+        <v>481735.070228666</v>
       </c>
     </row>
     <row r="196" spans="1:2">
-      <c r="A196" s="1" t="n">
+      <c r="A196" s="1">
         <v>194</v>
       </c>
-      <c r="B196" t="n">
-        <v>367045.059992591</v>
+      <c r="B196">
+        <v>511955.368199366</v>
       </c>
     </row>
     <row r="197" spans="1:2">
-      <c r="A197" s="1" t="n">
+      <c r="A197" s="1">
         <v>195</v>
       </c>
-      <c r="B197" t="n">
-        <v>357661.9741187847</v>
+      <c r="B197">
+        <v>500454.5247337151</v>
       </c>
     </row>
     <row r="198" spans="1:2">
-      <c r="A198" s="1" t="n">
+      <c r="A198" s="1">
         <v>196</v>
       </c>
-      <c r="B198" t="n">
-        <v>329328.4555707897</v>
+      <c r="B198">
+        <v>477121.0394866091</v>
       </c>
     </row>
     <row r="199" spans="1:2">
-      <c r="A199" s="1" t="n">
+      <c r="A199" s="1">
         <v>197</v>
       </c>
-      <c r="B199" t="n">
-        <v>316674.4794706317</v>
+      <c r="B199">
+        <v>469281.2957524483</v>
       </c>
     </row>
     <row r="200" spans="1:2">
-      <c r="A200" s="1" t="n">
+      <c r="A200" s="1">
         <v>198</v>
       </c>
-      <c r="B200" t="n">
-        <v>293035.6178640242</v>
+      <c r="B200">
+        <v>444712.4955223093</v>
       </c>
     </row>
     <row r="201" spans="1:2">
-      <c r="A201" s="1" t="n">
+      <c r="A201" s="1">
         <v>199</v>
       </c>
-      <c r="B201" t="n">
-        <v>261289.6289702056</v>
+      <c r="B201">
+        <v>441677.7161233965</v>
       </c>
     </row>
     <row r="202" spans="1:2">
-      <c r="A202" s="1" t="n">
+      <c r="A202" s="1">
         <v>200</v>
       </c>
-      <c r="B202" t="n">
-        <v>277647.7231629873</v>
+      <c r="B202">
+        <v>421557.4822015171</v>
       </c>
     </row>
     <row r="203" spans="1:2">
-      <c r="A203" s="1" t="n">
+      <c r="A203" s="1">
         <v>201</v>
       </c>
-      <c r="B203" t="n">
-        <v>291237.8760379928</v>
+      <c r="B203">
+        <v>420462.0618795322</v>
       </c>
     </row>
     <row r="204" spans="1:2">
-      <c r="A204" s="1" t="n">
+      <c r="A204" s="1">
         <v>202</v>
       </c>
-      <c r="B204" t="n">
-        <v>297426.5051648295</v>
+      <c r="B204">
+        <v>412278.272226038</v>
       </c>
     </row>
     <row r="205" spans="1:2">
-      <c r="A205" s="1" t="n">
+      <c r="A205" s="1">
         <v>203</v>
       </c>
-      <c r="B205" t="n">
-        <v>269971.3183564785</v>
+      <c r="B205">
+        <v>405740.5173984842</v>
       </c>
     </row>
     <row r="206" spans="1:2">
-      <c r="A206" s="1" t="n">
+      <c r="A206" s="1">
         <v>204</v>
       </c>
-      <c r="B206" t="n">
-        <v>251643.2131670181</v>
+      <c r="B206">
+        <v>402150.8415346429</v>
       </c>
     </row>
     <row r="207" spans="1:2">
-      <c r="A207" s="1" t="n">
+      <c r="A207" s="1">
         <v>205</v>
       </c>
-      <c r="B207" t="n">
-        <v>268465.8038998595</v>
+      <c r="B207">
+        <v>395737.017743455</v>
       </c>
     </row>
     <row r="208" spans="1:2">
-      <c r="A208" s="1" t="n">
+      <c r="A208" s="1">
         <v>206</v>
       </c>
-      <c r="B208" t="n">
-        <v>256839.7103444016</v>
+      <c r="B208">
+        <v>392531.3984622968</v>
       </c>
     </row>
     <row r="209" spans="1:2">
-      <c r="A209" s="1" t="n">
+      <c r="A209" s="1">
         <v>207</v>
       </c>
-      <c r="B209" t="n">
-        <v>251573.7634480014</v>
+      <c r="B209">
+        <v>407763.0151746356</v>
       </c>
     </row>
     <row r="210" spans="1:2">
-      <c r="A210" s="1" t="n">
+      <c r="A210" s="1">
         <v>208</v>
       </c>
-      <c r="B210" t="n">
-        <v>250759.0532966536</v>
+      <c r="B210">
+        <v>403277.3269452521</v>
       </c>
     </row>
     <row r="211" spans="1:2">
-      <c r="A211" s="1" t="n">
+      <c r="A211" s="1">
         <v>209</v>
       </c>
-      <c r="B211" t="n">
-        <v>265188.6565350045</v>
+      <c r="B211">
+        <v>395358.0425841144</v>
       </c>
     </row>
     <row r="212" spans="1:2">
-      <c r="A212" s="1" t="n">
+      <c r="A212" s="1">
         <v>210</v>
       </c>
-      <c r="B212" t="n">
-        <v>266795.3582717639</v>
+      <c r="B212">
+        <v>370729.591633044</v>
       </c>
     </row>
     <row r="213" spans="1:2">
-      <c r="A213" s="1" t="n">
+      <c r="A213" s="1">
         <v>211</v>
       </c>
-      <c r="B213" t="n">
-        <v>245538.0324621675</v>
+      <c r="B213">
+        <v>366919.1819848929</v>
       </c>
     </row>
     <row r="214" spans="1:2">
-      <c r="A214" s="1" t="n">
+      <c r="A214" s="1">
         <v>212</v>
       </c>
-      <c r="B214" t="n">
-        <v>230526.6771046789</v>
+      <c r="B214">
+        <v>350632.2275197252</v>
       </c>
     </row>
     <row r="215" spans="1:2">
-      <c r="A215" s="1" t="n">
+      <c r="A215" s="1">
         <v>213</v>
       </c>
-      <c r="B215" t="n">
-        <v>246742.0101199752</v>
+      <c r="B215">
+        <v>300538.8859283043</v>
       </c>
     </row>
     <row r="216" spans="1:2">
-      <c r="A216" s="1" t="n">
+      <c r="A216" s="1">
         <v>214</v>
       </c>
-      <c r="B216" t="n">
-        <v>258396.0941619172</v>
+      <c r="B216">
+        <v>295463.6230979101</v>
       </c>
     </row>
     <row r="217" spans="1:2">
-      <c r="A217" s="1" t="n">
+      <c r="A217" s="1">
         <v>215</v>
       </c>
-      <c r="B217" t="n">
-        <v>228877.9731721168</v>
+      <c r="B217">
+        <v>286308.5879821563</v>
       </c>
     </row>
     <row r="218" spans="1:2">
-      <c r="A218" s="1" t="n">
+      <c r="A218" s="1">
         <v>216</v>
       </c>
-      <c r="B218" t="n">
-        <v>235318.6282944455</v>
+      <c r="B218">
+        <v>278993.6692907497</v>
       </c>
     </row>
     <row r="219" spans="1:2">
-      <c r="A219" s="1" t="n">
+      <c r="A219" s="1">
         <v>217</v>
       </c>
-      <c r="B219" t="n">
-        <v>228587.3978004697</v>
+      <c r="B219">
+        <v>280814.3456314473</v>
       </c>
     </row>
     <row r="220" spans="1:2">
-      <c r="A220" s="1" t="n">
+      <c r="A220" s="1">
         <v>218</v>
       </c>
-      <c r="B220" t="n">
-        <v>219015.2684409558</v>
+      <c r="B220">
+        <v>278859.4214288148</v>
       </c>
     </row>
     <row r="221" spans="1:2">
-      <c r="A221" s="1" t="n">
+      <c r="A221" s="1">
         <v>219</v>
       </c>
-      <c r="B221" t="n">
-        <v>198157.3432569983</v>
+      <c r="B221">
+        <v>269668.9038932275</v>
       </c>
     </row>
     <row r="222" spans="1:2">
-      <c r="A222" s="1" t="n">
+      <c r="A222" s="1">
         <v>220</v>
       </c>
-      <c r="B222" t="n">
-        <v>197560.0011899701</v>
+      <c r="B222">
+        <v>266445.486302954</v>
       </c>
     </row>
     <row r="223" spans="1:2">
-      <c r="A223" s="1" t="n">
+      <c r="A223" s="1">
         <v>221</v>
       </c>
-      <c r="B223" t="n">
-        <v>188748.3825104404</v>
+      <c r="B223">
+        <v>268924.1318956148</v>
       </c>
     </row>
     <row r="224" spans="1:2">
-      <c r="A224" s="1" t="n">
+      <c r="A224" s="1">
         <v>222</v>
       </c>
-      <c r="B224" t="n">
-        <v>179117.759212128</v>
+      <c r="B224">
+        <v>278930.0918279239</v>
       </c>
     </row>
     <row r="225" spans="1:2">
-      <c r="A225" s="1" t="n">
+      <c r="A225" s="1">
         <v>223</v>
       </c>
-      <c r="B225" t="n">
-        <v>188881.1333239427</v>
+      <c r="B225">
+        <v>289856.7134180432</v>
       </c>
     </row>
     <row r="226" spans="1:2">
-      <c r="A226" s="1" t="n">
+      <c r="A226" s="1">
         <v>224</v>
       </c>
-      <c r="B226" t="n">
-        <v>204079.4357366434</v>
+      <c r="B226">
+        <v>301605.6203513335</v>
       </c>
     </row>
     <row r="227" spans="1:2">
-      <c r="A227" s="1" t="n">
+      <c r="A227" s="1">
         <v>225</v>
       </c>
-      <c r="B227" t="n">
-        <v>258915.0119033571</v>
+      <c r="B227">
+        <v>304398.1915821711</v>
       </c>
     </row>
     <row r="228" spans="1:2">
-      <c r="A228" s="1" t="n">
+      <c r="A228" s="1">
         <v>226</v>
       </c>
-      <c r="B228" t="n">
-        <v>247268.4176602963</v>
+      <c r="B228">
+        <v>265758.6947629285</v>
       </c>
     </row>
     <row r="229" spans="1:2">
-      <c r="A229" s="1" t="n">
+      <c r="A229" s="1">
         <v>227</v>
       </c>
-      <c r="B229" t="n">
-        <v>301412.0055257032</v>
+      <c r="B229">
+        <v>264938.3814163383</v>
       </c>
     </row>
     <row r="230" spans="1:2">
-      <c r="A230" s="1" t="n">
+      <c r="A230" s="1">
         <v>228</v>
       </c>
-      <c r="B230" t="n">
-        <v>297862.6704159107</v>
+      <c r="B230">
+        <v>261955.4344577711</v>
       </c>
     </row>
     <row r="231" spans="1:2">
-      <c r="A231" s="1" t="n">
+      <c r="A231" s="1">
         <v>229</v>
       </c>
-      <c r="B231" t="n">
-        <v>288690.1241529262</v>
+      <c r="B231">
+        <v>264276.7685163571</v>
       </c>
     </row>
     <row r="232" spans="1:2">
-      <c r="A232" s="1" t="n">
+      <c r="A232" s="1">
         <v>230</v>
       </c>
-      <c r="B232" t="n">
-        <v>280434.6658798804</v>
+      <c r="B232">
+        <v>312578.7820170429</v>
       </c>
     </row>
     <row r="233" spans="1:2">
-      <c r="A233" s="1" t="n">
+      <c r="A233" s="1">
         <v>231</v>
       </c>
-      <c r="B233" t="n">
-        <v>283156.9568598267</v>
+      <c r="B233">
+        <v>290978.1030483287</v>
       </c>
     </row>
     <row r="234" spans="1:2">
-      <c r="A234" s="1" t="n">
+      <c r="A234" s="1">
         <v>232</v>
       </c>
-      <c r="B234" t="n">
-        <v>268714.7001354136</v>
+      <c r="B234">
+        <v>296101.9326909706</v>
       </c>
     </row>
     <row r="235" spans="1:2">
-      <c r="A235" s="1" t="n">
+      <c r="A235" s="1">
         <v>233</v>
       </c>
-      <c r="B235" t="n">
-        <v>269249.9907135956</v>
+      <c r="B235">
+        <v>289911.8229413797</v>
       </c>
     </row>
     <row r="236" spans="1:2">
-      <c r="A236" s="1" t="n">
+      <c r="A236" s="1">
         <v>234</v>
       </c>
-      <c r="B236" t="n">
-        <v>271928.8193838806</v>
+      <c r="B236">
+        <v>293501.2829717943</v>
       </c>
     </row>
     <row r="237" spans="1:2">
-      <c r="A237" s="1" t="n">
+      <c r="A237" s="1">
         <v>235</v>
       </c>
-      <c r="B237" t="n">
-        <v>263372.4628508802</v>
+      <c r="B237">
+        <v>298568.9503645692</v>
       </c>
     </row>
     <row r="238" spans="1:2">
-      <c r="A238" s="1" t="n">
+      <c r="A238" s="1">
         <v>236</v>
       </c>
-      <c r="B238" t="n">
-        <v>266650.8876648851</v>
+      <c r="B238">
+        <v>300921.0268675716</v>
       </c>
     </row>
     <row r="239" spans="1:2">
-      <c r="A239" s="1" t="n">
+      <c r="A239" s="1">
         <v>237</v>
       </c>
-      <c r="B239" t="n">
-        <v>278054.4761351036</v>
+      <c r="B239">
+        <v>309582.3699901745</v>
       </c>
     </row>
     <row r="240" spans="1:2">
-      <c r="A240" s="1" t="n">
+      <c r="A240" s="1">
         <v>238</v>
       </c>
-      <c r="B240" t="n">
-        <v>300643.3370002452</v>
+      <c r="B240">
+        <v>312965.3462176333</v>
       </c>
     </row>
     <row r="241" spans="1:2">
-      <c r="A241" s="1" t="n">
+      <c r="A241" s="1">
         <v>239</v>
       </c>
-      <c r="B241" t="n">
-        <v>307455.3752980439</v>
+      <c r="B241">
+        <v>307748.8745801271</v>
       </c>
     </row>
     <row r="242" spans="1:2">
-      <c r="A242" s="1" t="n">
+      <c r="A242" s="1">
         <v>240</v>
       </c>
-      <c r="B242" t="n">
-        <v>299462.252467285</v>
+      <c r="B242">
+        <v>298764.8028803919</v>
       </c>
     </row>
     <row r="243" spans="1:2">
-      <c r="A243" s="1" t="n">
+      <c r="A243" s="1">
         <v>241</v>
       </c>
-      <c r="B243" t="n">
-        <v>272876.2241624391</v>
+      <c r="B243">
+        <v>296569.5609463981</v>
       </c>
     </row>
     <row r="244" spans="1:2">
-      <c r="A244" s="1" t="n">
+      <c r="A244" s="1">
         <v>242</v>
       </c>
-      <c r="B244" t="n">
-        <v>318733.098602566</v>
+      <c r="B244">
+        <v>347754.4340018969</v>
       </c>
     </row>
     <row r="245" spans="1:2">
-      <c r="A245" s="1" t="n">
+      <c r="A245" s="1">
         <v>243</v>
       </c>
-      <c r="B245" t="n">
-        <v>247861.7519773121</v>
+      <c r="B245">
+        <v>273668.0839782676</v>
       </c>
     </row>
     <row r="246" spans="1:2">
-      <c r="A246" s="1" t="n">
+      <c r="A246" s="1">
         <v>244</v>
       </c>
-      <c r="B246" t="n">
-        <v>252597.1818475446</v>
+      <c r="B246">
+        <v>271709.2385409841</v>
       </c>
     </row>
     <row r="247" spans="1:2">
-      <c r="A247" s="1" t="n">
+      <c r="A247" s="1">
         <v>245</v>
       </c>
-      <c r="B247" t="n">
-        <v>248906.665073445</v>
+      <c r="B247">
+        <v>239160.0467949053</v>
       </c>
     </row>
     <row r="248" spans="1:2">
-      <c r="A248" s="1" t="n">
+      <c r="A248" s="1">
         <v>246</v>
       </c>
-      <c r="B248" t="n">
-        <v>246005.1513794877</v>
+      <c r="B248">
+        <v>243111.6017963083</v>
       </c>
     </row>
     <row r="249" spans="1:2">
-      <c r="A249" s="1" t="n">
+      <c r="A249" s="1">
         <v>247</v>
       </c>
-      <c r="B249" t="n">
-        <v>242403.0067445032</v>
+      <c r="B249">
+        <v>243576.744400431</v>
       </c>
     </row>
     <row r="250" spans="1:2">
-      <c r="A250" s="1" t="n">
+      <c r="A250" s="1">
         <v>248</v>
       </c>
-      <c r="B250" t="n">
-        <v>253165.6266935841</v>
+      <c r="B250">
+        <v>236281.2336227557</v>
       </c>
     </row>
     <row r="251" spans="1:2">
-      <c r="A251" s="1" t="n">
+      <c r="A251" s="1">
         <v>249</v>
       </c>
-      <c r="B251" t="n">
-        <v>250806.031410518</v>
+      <c r="B251">
+        <v>223686.8167526035</v>
       </c>
     </row>
     <row r="252" spans="1:2">
-      <c r="A252" s="1" t="n">
+      <c r="A252" s="1">
         <v>250</v>
       </c>
-      <c r="B252" t="n">
-        <v>231931.176511858</v>
+      <c r="B252">
+        <v>211633.0337334838</v>
       </c>
     </row>
     <row r="253" spans="1:2">
-      <c r="A253" s="1" t="n">
+      <c r="A253" s="1">
         <v>251</v>
       </c>
-      <c r="B253" t="n">
-        <v>256127.3312189652</v>
+      <c r="B253">
+        <v>202684.0494694508</v>
       </c>
     </row>
     <row r="254" spans="1:2">
-      <c r="A254" s="1" t="n">
+      <c r="A254" s="1">
         <v>252</v>
       </c>
-      <c r="B254" t="n">
-        <v>234000.4873575443</v>
+      <c r="B254">
+        <v>212111.4645950212</v>
       </c>
     </row>
     <row r="255" spans="1:2">
-      <c r="A255" s="1" t="n">
+      <c r="A255" s="1">
         <v>253</v>
       </c>
-      <c r="B255" t="n">
-        <v>219596.3821052063</v>
+      <c r="B255">
+        <v>197811.1609098373</v>
       </c>
     </row>
     <row r="256" spans="1:2">
-      <c r="A256" s="1" t="n">
+      <c r="A256" s="1">
         <v>254</v>
       </c>
-      <c r="B256" t="n">
-        <v>221883.485915507</v>
+      <c r="B256">
+        <v>212068.4375772933</v>
       </c>
     </row>
     <row r="257" spans="1:2">
-      <c r="A257" s="1" t="n">
+      <c r="A257" s="1">
         <v>255</v>
       </c>
-      <c r="B257" t="n">
-        <v>223364.5626772861</v>
+      <c r="B257">
+        <v>211782.675747424</v>
       </c>
     </row>
     <row r="258" spans="1:2">
-      <c r="A258" s="1" t="n">
+      <c r="A258" s="1">
         <v>256</v>
       </c>
-      <c r="B258" t="n">
-        <v>230792.3025010777</v>
+      <c r="B258">
+        <v>198609.9725227244</v>
       </c>
     </row>
     <row r="259" spans="1:2">
-      <c r="A259" s="1" t="n">
+      <c r="A259" s="1">
         <v>257</v>
       </c>
-      <c r="B259" t="n">
-        <v>230919.6802802178</v>
+      <c r="B259">
+        <v>214623.4365562866</v>
       </c>
     </row>
     <row r="260" spans="1:2">
-      <c r="A260" s="1" t="n">
+      <c r="A260" s="1">
         <v>258</v>
       </c>
-      <c r="B260" t="n">
-        <v>236428.2781523348</v>
+      <c r="B260">
+        <v>210155.6351940506</v>
       </c>
     </row>
     <row r="261" spans="1:2">
-      <c r="A261" s="1" t="n">
+      <c r="A261" s="1">
         <v>259</v>
       </c>
-      <c r="B261" t="n">
-        <v>244482.0763187392</v>
+      <c r="B261">
+        <v>206695.3894430898</v>
       </c>
     </row>
     <row r="262" spans="1:2">
-      <c r="A262" s="1" t="n">
+      <c r="A262" s="1">
         <v>260</v>
       </c>
-      <c r="B262" t="n">
-        <v>278118.8233614686</v>
+      <c r="B262">
+        <v>197684.4850873</v>
       </c>
     </row>
     <row r="263" spans="1:2">
-      <c r="A263" s="1" t="n">
+      <c r="A263" s="1">
         <v>261</v>
       </c>
-      <c r="B263" t="n">
-        <v>315290.3590219494</v>
+      <c r="B263">
+        <v>190628.9394990033</v>
       </c>
     </row>
     <row r="264" spans="1:2">
-      <c r="A264" s="1" t="n">
+      <c r="A264" s="1">
         <v>262</v>
       </c>
-      <c r="B264" t="n">
-        <v>320717.8429365511</v>
+      <c r="B264">
+        <v>188109.1174281992</v>
       </c>
     </row>
     <row r="265" spans="1:2">
-      <c r="A265" s="1" t="n">
+      <c r="A265" s="1">
         <v>263</v>
       </c>
-      <c r="B265" t="n">
-        <v>316003.4311584396</v>
+      <c r="B265">
+        <v>210078.0918835588</v>
       </c>
     </row>
     <row r="266" spans="1:2">
-      <c r="A266" s="1" t="n">
+      <c r="A266" s="1">
         <v>264</v>
       </c>
-      <c r="B266" t="n">
-        <v>292151.1620693259</v>
+      <c r="B266">
+        <v>209608.0106234914</v>
       </c>
     </row>
     <row r="267" spans="1:2">
-      <c r="A267" s="1" t="n">
+      <c r="A267" s="1">
         <v>265</v>
       </c>
-      <c r="B267" t="n">
-        <v>301274.5574435088</v>
+      <c r="B267">
+        <v>216329.6342574974</v>
       </c>
     </row>
     <row r="268" spans="1:2">
-      <c r="A268" s="1" t="n">
+      <c r="A268" s="1">
         <v>266</v>
       </c>
-      <c r="B268" t="n">
-        <v>281672.0498180473</v>
+      <c r="B268">
+        <v>213283.0894570964</v>
       </c>
     </row>
     <row r="269" spans="1:2">
-      <c r="A269" s="1" t="n">
+      <c r="A269" s="1">
         <v>267</v>
       </c>
-      <c r="B269" t="n">
-        <v>293100.164413297</v>
+      <c r="B269">
+        <v>212749.3166545677</v>
       </c>
     </row>
     <row r="270" spans="1:2">
-      <c r="A270" s="1" t="n">
+      <c r="A270" s="1">
         <v>268</v>
       </c>
-      <c r="B270" t="n">
-        <v>296201.8968468255</v>
+      <c r="B270">
+        <v>222409.1910845977</v>
       </c>
     </row>
     <row r="271" spans="1:2">
-      <c r="A271" s="1" t="n">
+      <c r="A271" s="1">
         <v>269</v>
       </c>
-      <c r="B271" t="n">
-        <v>282681.5522148052</v>
+      <c r="B271">
+        <v>217830.8011558902</v>
       </c>
     </row>
     <row r="272" spans="1:2">
-      <c r="A272" s="1" t="n">
+      <c r="A272" s="1">
         <v>270</v>
       </c>
-      <c r="B272" t="n">
-        <v>283098.5764479331</v>
+      <c r="B272">
+        <v>216767.3384239442</v>
       </c>
     </row>
     <row r="273" spans="1:2">
-      <c r="A273" s="1" t="n">
+      <c r="A273" s="1">
         <v>271</v>
       </c>
-      <c r="B273" t="n">
-        <v>292722.8681722545</v>
+      <c r="B273">
+        <v>203693.1368671907</v>
       </c>
     </row>
     <row r="274" spans="1:2">
-      <c r="A274" s="1" t="n">
+      <c r="A274" s="1">
         <v>272</v>
       </c>
-      <c r="B274" t="n">
-        <v>286939.506715568</v>
+      <c r="B274">
+        <v>210388.3002732337</v>
       </c>
     </row>
     <row r="275" spans="1:2">
-      <c r="A275" s="1" t="n">
+      <c r="A275" s="1">
         <v>273</v>
       </c>
-      <c r="B275" t="n">
-        <v>281063.8238236287</v>
+      <c r="B275">
+        <v>210775.90533652</v>
       </c>
     </row>
     <row r="276" spans="1:2">
-      <c r="A276" s="1" t="n">
+      <c r="A276" s="1">
         <v>274</v>
       </c>
-      <c r="B276" t="n">
-        <v>285450.8936223842</v>
+      <c r="B276">
+        <v>233273.4684058546</v>
       </c>
     </row>
     <row r="277" spans="1:2">
-      <c r="A277" s="1" t="n">
+      <c r="A277" s="1">
         <v>275</v>
       </c>
-      <c r="B277" t="n">
-        <v>271362.663090398</v>
+      <c r="B277">
+        <v>230301.322787267</v>
       </c>
     </row>
     <row r="278" spans="1:2">
-      <c r="A278" s="1" t="n">
+      <c r="A278" s="1">
         <v>276</v>
       </c>
-      <c r="B278" t="n">
-        <v>265274.2381514023</v>
+      <c r="B278">
+        <v>238217.4542927718</v>
       </c>
     </row>
     <row r="279" spans="1:2">
-      <c r="A279" s="1" t="n">
+      <c r="A279" s="1">
         <v>277</v>
       </c>
-      <c r="B279" t="n">
-        <v>279064.8120894546</v>
+      <c r="B279">
+        <v>239033.6851447316</v>
       </c>
     </row>
     <row r="280" spans="1:2">
-      <c r="A280" s="1" t="n">
+      <c r="A280" s="1">
         <v>278</v>
       </c>
-      <c r="B280" t="n">
-        <v>279866.3697742951</v>
+      <c r="B280">
+        <v>238685.2196023907</v>
       </c>
     </row>
     <row r="281" spans="1:2">
-      <c r="A281" s="1" t="n">
+      <c r="A281" s="1">
         <v>279</v>
       </c>
-      <c r="B281" t="n">
-        <v>283757.751999416</v>
+      <c r="B281">
+        <v>237925.9099433523</v>
       </c>
     </row>
     <row r="282" spans="1:2">
-      <c r="A282" s="1" t="n">
+      <c r="A282" s="1">
         <v>280</v>
       </c>
-      <c r="B282" t="n">
-        <v>268164.9772533056</v>
+      <c r="B282">
+        <v>237619.0828421348</v>
       </c>
     </row>
     <row r="283" spans="1:2">
-      <c r="A283" s="1" t="n">
+      <c r="A283" s="1">
         <v>281</v>
       </c>
-      <c r="B283" t="n">
-        <v>258214.7121787136</v>
+      <c r="B283">
+        <v>233058.2056785347</v>
       </c>
     </row>
     <row r="284" spans="1:2">
-      <c r="A284" s="1" t="n">
+      <c r="A284" s="1">
         <v>282</v>
       </c>
-      <c r="B284" t="n">
-        <v>266785.4426622574</v>
+      <c r="B284">
+        <v>232087.7013686394</v>
       </c>
     </row>
     <row r="285" spans="1:2">
-      <c r="A285" s="1" t="n">
+      <c r="A285" s="1">
         <v>283</v>
       </c>
-      <c r="B285" t="n">
-        <v>272489.0021342832</v>
+      <c r="B285">
+        <v>241379.5928926225</v>
       </c>
     </row>
     <row r="286" spans="1:2">
-      <c r="A286" s="1" t="n">
+      <c r="A286" s="1">
         <v>284</v>
       </c>
-      <c r="B286" t="n">
-        <v>280500.5352537589</v>
+      <c r="B286">
+        <v>234517.2747726373</v>
       </c>
     </row>
     <row r="287" spans="1:2">
-      <c r="A287" s="1" t="n">
+      <c r="A287" s="1">
         <v>285</v>
       </c>
-      <c r="B287" t="n">
-        <v>317597.2525342869</v>
+      <c r="B287">
+        <v>230242.256731449</v>
       </c>
     </row>
     <row r="288" spans="1:2">
-      <c r="A288" s="1" t="n">
+      <c r="A288" s="1">
         <v>286</v>
       </c>
-      <c r="B288" t="n">
-        <v>314615.3808643527</v>
+      <c r="B288">
+        <v>223495.1272607772</v>
       </c>
     </row>
     <row r="289" spans="1:2">
-      <c r="A289" s="1" t="n">
+      <c r="A289" s="1">
         <v>287</v>
       </c>
-      <c r="B289" t="n">
-        <v>310916.3413266849</v>
+      <c r="B289">
+        <v>234029.7653012383</v>
       </c>
     </row>
     <row r="290" spans="1:2">
-      <c r="A290" s="1" t="n">
+      <c r="A290" s="1">
         <v>288</v>
       </c>
-      <c r="B290" t="n">
-        <v>315143.453156497</v>
+      <c r="B290">
+        <v>223671.50209362</v>
       </c>
     </row>
     <row r="291" spans="1:2">
-      <c r="A291" s="1" t="n">
+      <c r="A291" s="1">
         <v>289</v>
       </c>
-      <c r="B291" t="n">
-        <v>292981.7312148895</v>
+      <c r="B291">
+        <v>220888.6057243255</v>
       </c>
     </row>
     <row r="292" spans="1:2">
-      <c r="A292" s="1" t="n">
+      <c r="A292" s="1">
         <v>290</v>
       </c>
-      <c r="B292" t="n">
-        <v>286798.3700541275</v>
+      <c r="B292">
+        <v>229133.3595800287</v>
       </c>
     </row>
     <row r="293" spans="1:2">
-      <c r="A293" s="1" t="n">
+      <c r="A293" s="1">
         <v>291</v>
       </c>
-      <c r="B293" t="n">
-        <v>298375.5770529342</v>
+      <c r="B293">
+        <v>230701.2530220088</v>
       </c>
     </row>
     <row r="294" spans="1:2">
-      <c r="A294" s="1" t="n">
+      <c r="A294" s="1">
         <v>292</v>
       </c>
-      <c r="B294" t="n">
-        <v>286556.9493170758</v>
+      <c r="B294">
+        <v>228887.042561033</v>
       </c>
     </row>
     <row r="295" spans="1:2">
-      <c r="A295" s="1" t="n">
+      <c r="A295" s="1">
         <v>293</v>
       </c>
-      <c r="B295" t="n">
-        <v>307520.9108448675</v>
+      <c r="B295">
+        <v>227895.7771673168</v>
       </c>
     </row>
     <row r="296" spans="1:2">
-      <c r="A296" s="1" t="n">
+      <c r="A296" s="1">
         <v>294</v>
       </c>
-      <c r="B296" t="n">
-        <v>294483.0350500659</v>
+      <c r="B296">
+        <v>233969.9525359409</v>
       </c>
     </row>
     <row r="297" spans="1:2">
-      <c r="A297" s="1" t="n">
+      <c r="A297" s="1">
         <v>295</v>
       </c>
-      <c r="B297" t="n">
-        <v>291103.3461735006</v>
+      <c r="B297">
+        <v>254014.712725957</v>
       </c>
     </row>
     <row r="298" spans="1:2">
-      <c r="A298" s="1" t="n">
+      <c r="A298" s="1">
         <v>296</v>
       </c>
-      <c r="B298" t="n">
-        <v>293141.2307016165</v>
+      <c r="B298">
+        <v>248015.9853713684</v>
       </c>
     </row>
     <row r="299" spans="1:2">
-      <c r="A299" s="1" t="n">
+      <c r="A299" s="1">
         <v>297</v>
       </c>
-      <c r="B299" t="n">
-        <v>287823.6909608018</v>
+      <c r="B299">
+        <v>238165.9661927305</v>
       </c>
     </row>
     <row r="300" spans="1:2">
-      <c r="A300" s="1" t="n">
+      <c r="A300" s="1">
         <v>298</v>
       </c>
-      <c r="B300" t="n">
-        <v>289832.4640420972</v>
+      <c r="B300">
+        <v>232042.5263743989</v>
       </c>
     </row>
     <row r="301" spans="1:2">
-      <c r="A301" s="1" t="n">
+      <c r="A301" s="1">
         <v>299</v>
       </c>
-      <c r="B301" t="n">
-        <v>283442.8265706992</v>
+      <c r="B301">
+        <v>240977.5563114067</v>
       </c>
     </row>
     <row r="302" spans="1:2">
-      <c r="A302" s="1" t="n">
+      <c r="A302" s="1">
         <v>300</v>
       </c>
-      <c r="B302" t="n">
-        <v>288967.9662909484</v>
+      <c r="B302">
+        <v>243701.8059527543</v>
       </c>
     </row>
     <row r="303" spans="1:2">
-      <c r="A303" s="1" t="n">
+      <c r="A303" s="1">
         <v>301</v>
       </c>
-      <c r="B303" t="n">
-        <v>290077.6437085447</v>
+      <c r="B303">
+        <v>238126.6947051177</v>
       </c>
     </row>
     <row r="304" spans="1:2">
-      <c r="A304" s="1" t="n">
+      <c r="A304" s="1">
         <v>302</v>
       </c>
-      <c r="B304" t="n">
-        <v>290124.2364964561</v>
+      <c r="B304">
+        <v>233108.3284587735</v>
       </c>
     </row>
     <row r="305" spans="1:2">
-      <c r="A305" s="1" t="n">
+      <c r="A305" s="1">
         <v>303</v>
       </c>
-      <c r="B305" t="n">
-        <v>314094.6536851682</v>
+      <c r="B305">
+        <v>241950.097853935</v>
       </c>
     </row>
     <row r="306" spans="1:2">
-      <c r="A306" s="1" t="n">
+      <c r="A306" s="1">
         <v>304</v>
       </c>
-      <c r="B306" t="n">
-        <v>299446.9291469132</v>
+      <c r="B306">
+        <v>271000.533373181</v>
       </c>
     </row>
     <row r="307" spans="1:2">
-      <c r="A307" s="1" t="n">
+      <c r="A307" s="1">
         <v>305</v>
       </c>
-      <c r="B307" t="n">
-        <v>297311.9295321113</v>
+      <c r="B307">
+        <v>235857.3118849632</v>
       </c>
     </row>
     <row r="308" spans="1:2">
-      <c r="A308" s="1" t="n">
+      <c r="A308" s="1">
         <v>306</v>
       </c>
-      <c r="B308" t="n">
-        <v>314288.3418478033</v>
+      <c r="B308">
+        <v>248014.5680109795</v>
       </c>
     </row>
     <row r="309" spans="1:2">
-      <c r="A309" s="1" t="n">
+      <c r="A309" s="1">
         <v>307</v>
       </c>
-      <c r="B309" t="n">
-        <v>307313.3121204323</v>
+      <c r="B309">
+        <v>285616.1634070312</v>
       </c>
     </row>
     <row r="310" spans="1:2">
-      <c r="A310" s="1" t="n">
+      <c r="A310" s="1">
         <v>308</v>
       </c>
-      <c r="B310" t="n">
-        <v>300828.3248296617</v>
+      <c r="B310">
+        <v>327472.49649106</v>
       </c>
     </row>
     <row r="311" spans="1:2">
-      <c r="A311" s="1" t="n">
+      <c r="A311" s="1">
         <v>309</v>
       </c>
-      <c r="B311" t="n">
-        <v>294030.4866007433</v>
+      <c r="B311">
+        <v>315161.1745550619</v>
       </c>
     </row>
     <row r="312" spans="1:2">
-      <c r="A312" s="1" t="n">
+      <c r="A312" s="1">
         <v>310</v>
       </c>
-      <c r="B312" t="n">
-        <v>293680.2148064134</v>
+      <c r="B312">
+        <v>301229.2769840794</v>
       </c>
     </row>
     <row r="313" spans="1:2">
-      <c r="A313" s="1" t="n">
+      <c r="A313" s="1">
         <v>311</v>
       </c>
-      <c r="B313" t="n">
-        <v>284929.3805572417</v>
+      <c r="B313">
+        <v>302027.9610906667</v>
       </c>
     </row>
     <row r="314" spans="1:2">
-      <c r="A314" s="1" t="n">
+      <c r="A314" s="1">
         <v>312</v>
       </c>
-      <c r="B314" t="n">
-        <v>306933.8114120438</v>
+      <c r="B314">
+        <v>281185.2711296779</v>
       </c>
     </row>
     <row r="315" spans="1:2">
-      <c r="A315" s="1" t="n">
+      <c r="A315" s="1">
         <v>313</v>
       </c>
-      <c r="B315" t="n">
-        <v>318626.7445297957</v>
+      <c r="B315">
+        <v>274545.5214897158</v>
       </c>
     </row>
     <row r="316" spans="1:2">
-      <c r="A316" s="1" t="n">
+      <c r="A316" s="1">
         <v>314</v>
       </c>
-      <c r="B316" t="n">
-        <v>319252.1052995613</v>
+      <c r="B316">
+        <v>273932.2646460043</v>
       </c>
     </row>
     <row r="317" spans="1:2">
-      <c r="A317" s="1" t="n">
+      <c r="A317" s="1">
         <v>315</v>
       </c>
-      <c r="B317" t="n">
-        <v>330353.275596905</v>
+      <c r="B317">
+        <v>292118.0969829845</v>
       </c>
     </row>
     <row r="318" spans="1:2">
-      <c r="A318" s="1" t="n">
+      <c r="A318" s="1">
         <v>316</v>
       </c>
-      <c r="B318" t="n">
-        <v>361196.9438611378</v>
+      <c r="B318">
+        <v>292245.5011767291</v>
       </c>
     </row>
     <row r="319" spans="1:2">
-      <c r="A319" s="1" t="n">
+      <c r="A319" s="1">
         <v>317</v>
       </c>
-      <c r="B319" t="n">
-        <v>331642.5312369833</v>
+      <c r="B319">
+        <v>290499.3907432615</v>
       </c>
     </row>
     <row r="320" spans="1:2">
-      <c r="A320" s="1" t="n">
+      <c r="A320" s="1">
         <v>318</v>
       </c>
-      <c r="B320" t="n">
-        <v>336390.9804738107</v>
+      <c r="B320">
+        <v>276456.7704624347</v>
       </c>
     </row>
     <row r="321" spans="1:2">
-      <c r="A321" s="1" t="n">
+      <c r="A321" s="1">
         <v>319</v>
       </c>
-      <c r="B321" t="n">
-        <v>328016.6961702953</v>
+      <c r="B321">
+        <v>298141.8017021908</v>
       </c>
     </row>
     <row r="322" spans="1:2">
-      <c r="A322" s="1" t="n">
+      <c r="A322" s="1">
         <v>320</v>
       </c>
-      <c r="B322" t="n">
-        <v>322900.9609450141</v>
+      <c r="B322">
+        <v>304402.1475052395</v>
       </c>
     </row>
     <row r="323" spans="1:2">
-      <c r="A323" s="1" t="n">
+      <c r="A323" s="1">
         <v>321</v>
       </c>
-      <c r="B323" t="n">
-        <v>317638.993975089</v>
+      <c r="B323">
+        <v>318971.7696105171</v>
       </c>
     </row>
     <row r="324" spans="1:2">
-      <c r="A324" s="1" t="n">
+      <c r="A324" s="1">
         <v>322</v>
       </c>
-      <c r="B324" t="n">
-        <v>308937.5335527988</v>
+      <c r="B324">
+        <v>307958.3325917181</v>
       </c>
     </row>
     <row r="325" spans="1:2">
-      <c r="A325" s="1" t="n">
+      <c r="A325" s="1">
         <v>323</v>
       </c>
-      <c r="B325" t="n">
-        <v>311714.5027858175</v>
+      <c r="B325">
+        <v>305952.8588923187</v>
       </c>
     </row>
     <row r="326" spans="1:2">
-      <c r="A326" s="1" t="n">
+      <c r="A326" s="1">
         <v>324</v>
       </c>
-      <c r="B326" t="n">
-        <v>300392.5012620004</v>
+      <c r="B326">
+        <v>294216.3727224536</v>
       </c>
     </row>
     <row r="327" spans="1:2">
-      <c r="A327" s="1" t="n">
+      <c r="A327" s="1">
         <v>325</v>
       </c>
-      <c r="B327" t="n">
-        <v>314132.6920019288</v>
+      <c r="B327">
+        <v>271534.4000616836</v>
       </c>
     </row>
     <row r="328" spans="1:2">
-      <c r="A328" s="1" t="n">
+      <c r="A328" s="1">
         <v>326</v>
       </c>
-      <c r="B328" t="n">
-        <v>340968.5520041193</v>
+      <c r="B328">
+        <v>271352.2436043367</v>
       </c>
     </row>
     <row r="329" spans="1:2">
-      <c r="A329" s="1" t="n">
+      <c r="A329" s="1">
         <v>327</v>
       </c>
-      <c r="B329" t="n">
-        <v>338565.0369419826</v>
+      <c r="B329">
+        <v>267561.4090701919</v>
       </c>
     </row>
     <row r="330" spans="1:2">
-      <c r="A330" s="1" t="n">
+      <c r="A330" s="1">
         <v>328</v>
       </c>
-      <c r="B330" t="n">
-        <v>344122.4439538243</v>
+      <c r="B330">
+        <v>279967.4461739713</v>
       </c>
     </row>
     <row r="331" spans="1:2">
-      <c r="A331" s="1" t="n">
+      <c r="A331" s="1">
         <v>329</v>
       </c>
-      <c r="B331" t="n">
-        <v>323144.1644988405</v>
+      <c r="B331">
+        <v>291112.0749987223</v>
       </c>
     </row>
     <row r="332" spans="1:2">
-      <c r="A332" s="1" t="n">
+      <c r="A332" s="1">
         <v>330</v>
       </c>
-      <c r="B332" t="n">
-        <v>318826.6679006178</v>
+      <c r="B332">
+        <v>262629.6421642564</v>
       </c>
     </row>
     <row r="333" spans="1:2">
-      <c r="A333" s="1" t="n">
+      <c r="A333" s="1">
         <v>331</v>
       </c>
-      <c r="B333" t="n">
-        <v>315166.2458607176</v>
+      <c r="B333">
+        <v>257567.9283682534</v>
       </c>
     </row>
     <row r="334" spans="1:2">
-      <c r="A334" s="1" t="n">
+      <c r="A334" s="1">
         <v>332</v>
       </c>
-      <c r="B334" t="n">
-        <v>306683.6884125606</v>
+      <c r="B334">
+        <v>253625.9768703801</v>
       </c>
     </row>
     <row r="335" spans="1:2">
-      <c r="A335" s="1" t="n">
+      <c r="A335" s="1">
         <v>333</v>
       </c>
-      <c r="B335" t="n">
-        <v>309582.3410811476</v>
+      <c r="B335">
+        <v>252247.9498350709</v>
       </c>
     </row>
     <row r="336" spans="1:2">
-      <c r="A336" s="1" t="n">
+      <c r="A336" s="1">
         <v>334</v>
       </c>
-      <c r="B336" t="n">
-        <v>325168.7935727648</v>
+      <c r="B336">
+        <v>244632.8719225523</v>
       </c>
     </row>
     <row r="337" spans="1:2">
-      <c r="A337" s="1" t="n">
+      <c r="A337" s="1">
         <v>335</v>
       </c>
-      <c r="B337" t="n">
-        <v>348396.328393293</v>
+      <c r="B337">
+        <v>259641.0527051871</v>
       </c>
     </row>
     <row r="338" spans="1:2">
-      <c r="A338" s="1" t="n">
+      <c r="A338" s="1">
         <v>336</v>
       </c>
-      <c r="B338" t="n">
-        <v>347627.7824816482</v>
+      <c r="B338">
+        <v>251360.5796639551</v>
       </c>
     </row>
     <row r="339" spans="1:2">
-      <c r="A339" s="1" t="n">
+      <c r="A339" s="1">
         <v>337</v>
       </c>
-      <c r="B339" t="n">
-        <v>365558.2122274079</v>
+      <c r="B339">
+        <v>247615.7392053487</v>
       </c>
     </row>
     <row r="340" spans="1:2">
-      <c r="A340" s="1" t="n">
+      <c r="A340" s="1">
         <v>338</v>
       </c>
-      <c r="B340" t="n">
-        <v>373852.5255182137</v>
+      <c r="B340">
+        <v>243975.3328910198</v>
       </c>
     </row>
     <row r="341" spans="1:2">
-      <c r="A341" s="1" t="n">
+      <c r="A341" s="1">
         <v>339</v>
       </c>
-      <c r="B341" t="n">
-        <v>381787.734677677</v>
+      <c r="B341">
+        <v>260829.3019584118</v>
       </c>
     </row>
     <row r="342" spans="1:2">
-      <c r="A342" s="1" t="n">
+      <c r="A342" s="1">
         <v>340</v>
       </c>
-      <c r="B342" t="n">
-        <v>375730.5477892361</v>
+      <c r="B342">
+        <v>270768.282772221</v>
       </c>
     </row>
     <row r="343" spans="1:2">
-      <c r="A343" s="1" t="n">
+      <c r="A343" s="1">
         <v>341</v>
       </c>
-      <c r="B343" t="n">
-        <v>370258.4704633839</v>
+      <c r="B343">
+        <v>278838.247431425</v>
       </c>
     </row>
     <row r="344" spans="1:2">
-      <c r="A344" s="1" t="n">
+      <c r="A344" s="1">
         <v>342</v>
       </c>
-      <c r="B344" t="n">
-        <v>419493.2247389095</v>
+      <c r="B344">
+        <v>284514.4864368422</v>
       </c>
     </row>
     <row r="345" spans="1:2">
-      <c r="A345" s="1" t="n">
+      <c r="A345" s="1">
         <v>343</v>
       </c>
-      <c r="B345" t="n">
-        <v>409926.9142061204</v>
+      <c r="B345">
+        <v>286315.6087407102</v>
       </c>
     </row>
     <row r="346" spans="1:2">
-      <c r="A346" s="1" t="n">
+      <c r="A346" s="1">
         <v>344</v>
       </c>
-      <c r="B346" t="n">
-        <v>423976.5655967939</v>
+      <c r="B346">
+        <v>299124.625146682</v>
       </c>
     </row>
     <row r="347" spans="1:2">
-      <c r="A347" s="1" t="n">
+      <c r="A347" s="1">
         <v>345</v>
       </c>
-      <c r="B347" t="n">
-        <v>450605.0266595364</v>
+      <c r="B347">
+        <v>303864.063068946</v>
       </c>
     </row>
     <row r="348" spans="1:2">
-      <c r="A348" s="1" t="n">
+      <c r="A348" s="1">
         <v>346</v>
       </c>
-      <c r="B348" t="n">
-        <v>432770.4520034528</v>
+      <c r="B348">
+        <v>330456.9072552212</v>
       </c>
     </row>
     <row r="349" spans="1:2">
-      <c r="A349" s="1" t="n">
+      <c r="A349" s="1">
         <v>347</v>
       </c>
-      <c r="B349" t="n">
-        <v>373223.0745880462</v>
+      <c r="B349">
+        <v>323824.7226278465</v>
       </c>
     </row>
     <row r="350" spans="1:2">
-      <c r="A350" s="1" t="n">
+      <c r="A350" s="1">
         <v>348</v>
       </c>
-      <c r="B350" t="n">
-        <v>371559.7212019249</v>
+      <c r="B350">
+        <v>307636.3771826634</v>
       </c>
     </row>
     <row r="351" spans="1:2">
-      <c r="A351" s="1" t="n">
+      <c r="A351" s="1">
         <v>349</v>
       </c>
-      <c r="B351" t="n">
-        <v>380585.1970968475</v>
+      <c r="B351">
+        <v>295849.4479567274</v>
       </c>
     </row>
     <row r="352" spans="1:2">
-      <c r="A352" s="1" t="n">
+      <c r="A352" s="1">
         <v>350</v>
       </c>
-      <c r="B352" t="n">
-        <v>380489.777819815</v>
+      <c r="B352">
+        <v>282792.4485403859</v>
       </c>
     </row>
     <row r="353" spans="1:2">
-      <c r="A353" s="1" t="n">
+      <c r="A353" s="1">
         <v>351</v>
       </c>
-      <c r="B353" t="n">
-        <v>347245.6704719832</v>
+      <c r="B353">
+        <v>275131.6962555808</v>
       </c>
     </row>
     <row r="354" spans="1:2">
-      <c r="A354" s="1" t="n">
+      <c r="A354" s="1">
         <v>352</v>
       </c>
-      <c r="B354" t="n">
-        <v>348825.6171748685</v>
+      <c r="B354">
+        <v>271420.3933764365</v>
       </c>
     </row>
     <row r="355" spans="1:2">
-      <c r="A355" s="1" t="n">
+      <c r="A355" s="1">
         <v>353</v>
       </c>
-      <c r="B355" t="n">
-        <v>339866.4964613447</v>
+      <c r="B355">
+        <v>275633.0983169181</v>
       </c>
     </row>
     <row r="356" spans="1:2">
-      <c r="A356" s="1" t="n">
+      <c r="A356" s="1">
         <v>354</v>
       </c>
-      <c r="B356" t="n">
-        <v>321333.9796318659</v>
+      <c r="B356">
+        <v>304755.5540764763</v>
       </c>
     </row>
     <row r="357" spans="1:2">
-      <c r="A357" s="1" t="n">
+      <c r="A357" s="1">
         <v>355</v>
       </c>
-      <c r="B357" t="n">
-        <v>316192.0975060489</v>
+      <c r="B357">
+        <v>285409.2311498214</v>
       </c>
     </row>
     <row r="358" spans="1:2">
-      <c r="A358" s="1" t="n">
+      <c r="A358" s="1">
         <v>356</v>
       </c>
-      <c r="B358" t="n">
-        <v>319207.4050782385</v>
+      <c r="B358">
+        <v>256976.9579759516</v>
       </c>
     </row>
     <row r="359" spans="1:2">
-      <c r="A359" s="1" t="n">
+      <c r="A359" s="1">
         <v>357</v>
       </c>
-      <c r="B359" t="n">
-        <v>326634.994286005</v>
+      <c r="B359">
+        <v>264660.779838454</v>
       </c>
     </row>
     <row r="360" spans="1:2">
-      <c r="A360" s="1" t="n">
+      <c r="A360" s="1">
         <v>358</v>
       </c>
-      <c r="B360" t="n">
-        <v>333817.276955273</v>
+      <c r="B360">
+        <v>254881.8874890123</v>
       </c>
     </row>
     <row r="361" spans="1:2">
-      <c r="A361" s="1" t="n">
+      <c r="A361" s="1">
         <v>359</v>
       </c>
-      <c r="B361" t="n">
-        <v>334558.152594528</v>
+      <c r="B361">
+        <v>271387.1453883781</v>
       </c>
     </row>
     <row r="362" spans="1:2">
-      <c r="A362" s="1" t="n">
+      <c r="A362" s="1">
         <v>360</v>
       </c>
-      <c r="B362" t="n">
-        <v>332311.6656626535</v>
+      <c r="B362">
+        <v>284402.7078929927</v>
       </c>
     </row>
     <row r="363" spans="1:2">
-      <c r="A363" s="1" t="n">
+      <c r="A363" s="1">
         <v>361</v>
       </c>
-      <c r="B363" t="n">
-        <v>318049.7053997361</v>
+      <c r="B363">
+        <v>303254.6860858632</v>
       </c>
     </row>
     <row r="364" spans="1:2">
-      <c r="A364" s="1" t="n">
+      <c r="A364" s="1">
         <v>362</v>
       </c>
-      <c r="B364" t="n">
-        <v>299930.5004972719</v>
+      <c r="B364">
+        <v>300305.3086566066</v>
       </c>
     </row>
     <row r="365" spans="1:2">
-      <c r="A365" s="1" t="n">
+      <c r="A365" s="1">
         <v>363</v>
       </c>
-      <c r="B365" t="n">
-        <v>287680.4110551605</v>
+      <c r="B365">
+        <v>314218.1660410424</v>
       </c>
     </row>
     <row r="366" spans="1:2">
-      <c r="A366" s="1" t="n">
+      <c r="A366" s="1">
         <v>364</v>
       </c>
-      <c r="B366" t="n">
-        <v>292788.6926980247</v>
+      <c r="B366">
+        <v>334159.6184309074</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>